<commit_message>
Added tree solving data
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Tree Generator.xlsx
+++ b/Dissertation/Research/Tree Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Will Garside\Documents\Projects\Active\CubeSolver\Dissertation\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CE5AF3-8A66-422A-9C63-1933E0833848}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7922333-832A-4CA9-A7E7-2DAF0653C3CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A08C0A5D-9DC9-4B70-9FA4-56456CBF2D01}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Depth</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>B R2 B2 R2 B2</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Growth</t>
   </si>
 </sst>
 </file>
@@ -114,13 +120,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -128,8 +131,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,237 +448,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0560A52-BF5A-499B-8B29-8C6B81E0205F}">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <f>G4-D4</f>
+        <v>3.1E-2</v>
+      </c>
+      <c r="J4" s="4">
+        <f>H4-E4</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>18</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>0.46700000000000003</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>261</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I9" si="0">G5-D5</f>
+        <v>0.41900000000000004</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J9" si="1">H5-E5</f>
+        <v>243</v>
+      </c>
+      <c r="K5" s="1">
+        <f>I5/I4</f>
+        <v>13.516129032258066</v>
+      </c>
+      <c r="L5" s="1">
+        <f>J5/J4</f>
+        <v>14.294117647058824</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.52200000000000002</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>262</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="2">
         <v>6.5449999999999999</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>3501</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0229999999999997</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>3239</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6:K9" si="2">I6/I5</f>
+        <v>14.37470167064439</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" ref="L6:L9" si="3">J6/J5</f>
+        <v>13.329218106995885</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>6.53</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>3502</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <v>87.323999999999998</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>46740</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>80.793999999999997</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="1"/>
+        <v>43238</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="2"/>
+        <v>13.414245392661465</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="3"/>
+        <v>13.349181846248841</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>86.903999999999996</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>46741</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="2">
+      <c r="G8" s="2">
+        <v>1149.732</v>
+      </c>
+      <c r="H8" s="1">
         <v>621648</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>1062.828</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>574907</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="2"/>
+        <v>13.154788721934798</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="3"/>
+        <v>13.296336555807391</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1165.3499999999999</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>621649</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>-1165.3499999999999</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>-621649</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.0964615158802742</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.081303584753708</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Small updates to code and more work to tex
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Tree Generator.xlsx
+++ b/Dissertation/Research/Tree Generator.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Projects\Active\CubeSolver\Dissertation\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Will Garside\Documents\Projects\Active\CubeSolver\Dissertation\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D741F0-DBC2-4547-A2A7-69B3AB35D415}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20207AD8-8616-4AE3-B178-A580ED48869C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{A08C0A5D-9DC9-4B70-9FA4-56456CBF2D01}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A08C0A5D-9DC9-4B70-9FA4-56456CBF2D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Graph" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Graph" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>Depth</t>
   </si>
@@ -97,6 +98,24 @@
   <si>
     <t>R2 B R2 B2 R2 B2</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Duplication Checked</t>
+  </si>
+  <si>
+    <t>All Positions</t>
+  </si>
+  <si>
+    <t>Dup:All Factor</t>
+  </si>
+  <si>
+    <t>Factor/Depth</t>
+  </si>
 </sst>
 </file>
 
@@ -161,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -176,12 +195,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -199,9 +212,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -209,6 +219,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2710,49 +2738,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0560A52-BF5A-499B-8B29-8C6B81E0205F}">
   <dimension ref="A2:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="E22:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="21.44140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="10" max="10" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2768,7 +2796,7 @@
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -2784,7 +2812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -2803,7 +2831,7 @@
       <c r="G4" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>17</v>
       </c>
       <c r="I4" s="2">
@@ -2815,7 +2843,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -2834,7 +2862,7 @@
       <c r="G5" s="2">
         <v>0.46700000000000003</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>261</v>
       </c>
       <c r="I5" s="2">
@@ -2854,7 +2882,7 @@
         <v>14.294117647058824</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -2873,7 +2901,7 @@
       <c r="G6" s="2">
         <v>6.5449999999999999</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>3501</v>
       </c>
       <c r="I6" s="2">
@@ -2894,7 +2922,7 @@
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -2913,7 +2941,7 @@
       <c r="G7" s="2">
         <v>87.323999999999998</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>46740</v>
       </c>
       <c r="I7" s="2">
@@ -2934,7 +2962,7 @@
       </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -2953,7 +2981,7 @@
       <c r="G8" s="2">
         <v>1149.732</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>621648</v>
       </c>
       <c r="I8" s="2">
@@ -2974,7 +3002,7 @@
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2991,14 +3019,14 @@
         <v>22</v>
       </c>
       <c r="G9" s="2">
-        <v>14750</v>
-      </c>
-      <c r="H9" s="11">
+        <v>15053.42</v>
+      </c>
+      <c r="H9" s="9">
         <v>8240086</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
-        <v>13584.65</v>
+        <v>13888.07</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="1"/>
@@ -3006,7 +3034,7 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>12.781607183852891</v>
+        <v>13.067090818081571</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
@@ -3014,74 +3042,74 @@
       </c>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <f>AVERAGE(K5:L9)</f>
-        <v>13.476192511172821</v>
-      </c>
-      <c r="B14" s="13" t="s">
+        <v>13.504740874595688</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="5" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5" t="s">
+      <c r="J16" s="14"/>
+      <c r="K16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
@@ -3091,7 +3119,7 @@
       <c r="G17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="9" t="s">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -3107,765 +3135,779 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="14">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="9">
+      <c r="C18" s="11"/>
+      <c r="D18" s="7">
         <f t="shared" ref="D18:E23" si="4">D4</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="9">
+      <c r="F18" s="11"/>
+      <c r="G18" s="7">
         <f t="shared" ref="G18:H23" si="5">G4</f>
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="12">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="7">
         <f>G18-D18</f>
         <v>3.1E-2</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="8">
         <f>H18-E18</f>
         <v>17</v>
       </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="14">
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
         <v>2</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="9">
+      <c r="C19" s="11"/>
+      <c r="D19" s="7">
         <f t="shared" si="4"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="9">
+      <c r="F19" s="11"/>
+      <c r="G19" s="7">
         <f t="shared" si="5"/>
         <v>0.46700000000000003</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="12">
         <f t="shared" si="5"/>
         <v>261</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="7">
         <f t="shared" ref="I19:I37" si="6">G19-D19</f>
         <v>0.41900000000000004</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <f t="shared" ref="J19:J37" si="7">H19-E19</f>
         <v>243</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="11">
         <f>I19/I18</f>
         <v>13.516129032258066</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="11">
         <f>J19/J18</f>
         <v>14.294117647058824</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="14">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
         <v>3</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="9">
+      <c r="C20" s="11"/>
+      <c r="D20" s="7">
         <f t="shared" si="4"/>
         <v>0.52200000000000002</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="8">
         <f t="shared" si="4"/>
         <v>262</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="9">
+      <c r="F20" s="11"/>
+      <c r="G20" s="7">
         <f t="shared" si="5"/>
         <v>6.5449999999999999</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="12">
         <f t="shared" si="5"/>
         <v>3501</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="7">
         <f t="shared" si="6"/>
         <v>6.0229999999999997</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="8">
         <f t="shared" si="7"/>
         <v>3239</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="11">
         <f t="shared" ref="K20:K37" si="8">I20/I19</f>
         <v>14.37470167064439</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="11">
         <f t="shared" ref="L20:L37" si="9">J20/J19</f>
         <v>13.329218106995885</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="14">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
         <v>4</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="9">
+      <c r="C21" s="11"/>
+      <c r="D21" s="7">
         <f t="shared" si="4"/>
         <v>6.53</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="8">
         <f t="shared" si="4"/>
         <v>3502</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="9">
+      <c r="F21" s="11"/>
+      <c r="G21" s="7">
         <f t="shared" si="5"/>
         <v>87.323999999999998</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="12">
         <f t="shared" si="5"/>
         <v>46740</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="7">
         <f t="shared" si="6"/>
         <v>80.793999999999997</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="8">
         <f t="shared" si="7"/>
         <v>43238</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="11">
         <f t="shared" si="8"/>
         <v>13.414245392661465</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="11">
         <f t="shared" si="9"/>
         <v>13.349181846248841</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="14">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
         <v>5</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="9">
+      <c r="C22" s="11"/>
+      <c r="D22" s="7">
         <f t="shared" si="4"/>
         <v>86.903999999999996</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="8">
         <f t="shared" si="4"/>
         <v>46741</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="9">
+      <c r="F22" s="11"/>
+      <c r="G22" s="7">
         <f t="shared" si="5"/>
         <v>1149.732</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="12">
         <f t="shared" si="5"/>
         <v>621648</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="7">
         <f t="shared" si="6"/>
         <v>1062.828</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="8">
         <f t="shared" si="7"/>
         <v>574907</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="11">
         <f t="shared" si="8"/>
         <v>13.154788721934798</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="11">
         <f t="shared" si="9"/>
         <v>13.296336555807391</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="14">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
         <v>6</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="9">
+      <c r="C23" s="11"/>
+      <c r="D23" s="7">
         <f t="shared" si="4"/>
         <v>1165.3499999999999</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="8">
         <f t="shared" si="4"/>
         <v>621649</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="9">
+      <c r="F23" s="11"/>
+      <c r="G23" s="7">
         <f t="shared" si="5"/>
-        <v>14750</v>
-      </c>
-      <c r="H23" s="15">
+        <v>15053.42</v>
+      </c>
+      <c r="H23" s="12">
         <f>H9</f>
         <v>8240086</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="7">
         <f t="shared" si="6"/>
-        <v>13584.65</v>
-      </c>
-      <c r="J23" s="10">
+        <v>13888.07</v>
+      </c>
+      <c r="J23" s="8">
         <f t="shared" si="7"/>
         <v>7618437</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="11">
         <f t="shared" si="8"/>
-        <v>12.781607183852891</v>
-      </c>
-      <c r="L23" s="14">
+        <v>13.067090818081571</v>
+      </c>
+      <c r="L23" s="11">
         <f t="shared" si="9"/>
         <v>13.251598954265646</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>7</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="18">
         <f>D23*$A$14</f>
-        <v>15704.480942895245</v>
-      </c>
-      <c r="E24" s="3">
+        <v>15737.749778210084</v>
+      </c>
+      <c r="E24" s="18">
         <f t="shared" ref="E24:E37" si="10">H23+1</f>
         <v>8240087</v>
       </c>
-      <c r="G24" s="2">
-        <f>G23*$A$14</f>
-        <v>198773.83953979911</v>
-      </c>
-      <c r="H24" s="11">
-        <f>H23*$A$14</f>
-        <v>111044985.24462001</v>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18">
+        <f t="shared" ref="G24:G37" si="11">G23*$A$14</f>
+        <v>203292.53637645624</v>
+      </c>
+      <c r="H24" s="19">
+        <f t="shared" ref="H24:H37" si="12">H23*$A$14</f>
+        <v>111280226.21438369</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="6"/>
-        <v>183069.35859690385</v>
+        <v>187554.78659824614</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="7"/>
-        <v>102804898.24462001</v>
+        <v>103040139.21438369</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="9"/>
-        <v>13.494224372350917</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.525102224299248</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>8</v>
       </c>
-      <c r="D25" s="2">
-        <f t="shared" ref="D25:D37" si="11">D24*$A$14</f>
-        <v>211636.60847450118</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="D25" s="18">
+        <f t="shared" ref="D25:D37" si="13">D24*$A$14</f>
+        <v>212534.23270395293</v>
+      </c>
+      <c r="E25" s="18">
         <f t="shared" si="10"/>
-        <v>111044986.24462001</v>
-      </c>
-      <c r="G25" s="2">
-        <f>G24*$A$14</f>
-        <v>2678714.5278233085</v>
-      </c>
-      <c r="H25" s="11">
-        <f>H24*$A$14</f>
-        <v>1496463598.5568445</v>
+        <v>111280227.21438369</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18">
+        <f t="shared" si="11"/>
+        <v>2745413.0255033593</v>
+      </c>
+      <c r="H25" s="19">
+        <f t="shared" si="12"/>
+        <v>1502810619.491642</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="6"/>
-        <v>2467077.9193488071</v>
+        <v>2532878.7927994062</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" si="7"/>
-        <v>1385418612.3122244</v>
+        <v>1391530392.2772584</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172819</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192632530777</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740995953647</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>9</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="18">
+        <f t="shared" si="13"/>
+        <v>2870219.7396479049</v>
+      </c>
+      <c r="E26" s="18">
+        <f t="shared" si="10"/>
+        <v>1502810620.491642</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18">
         <f t="shared" si="11"/>
-        <v>2852055.6782140872</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="10"/>
-        <v>1496463599.5568445</v>
-      </c>
-      <c r="G26" s="2">
-        <f>G25*$A$14</f>
-        <v>36098872.659422308</v>
-      </c>
-      <c r="H26" s="11">
-        <f>H25*$A$14</f>
-        <v>20166631540.114479</v>
+        <v>37076091.50316263</v>
+      </c>
+      <c r="H26" s="19">
+        <f t="shared" si="12"/>
+        <v>20295067999.825245</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="6"/>
-        <v>33246816.98120822</v>
+        <v>34205871.763514727</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" si="7"/>
-        <v>18670167940.557636</v>
+        <v>18792257379.333603</v>
       </c>
       <c r="K26" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.50474087459569</v>
       </c>
       <c r="L26" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192520178182</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740883582009</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>10</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="18">
+        <f t="shared" si="13"/>
+        <v>38761573.837094456</v>
+      </c>
+      <c r="E27" s="18">
+        <f t="shared" si="10"/>
+        <v>20295068000.825245</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18">
         <f t="shared" si="11"/>
-        <v>38434851.3721966</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="10"/>
-        <v>20166631541.114479</v>
-      </c>
-      <c r="G27" s="2">
-        <f>G26*$A$14</f>
-        <v>486475357.39468819</v>
-      </c>
-      <c r="H27" s="11">
-        <f>H26*$A$14</f>
-        <v>271769408936.47235</v>
+        <v>500703008.39301026</v>
+      </c>
+      <c r="H27" s="19">
+        <f t="shared" si="12"/>
+        <v>274079634369.93893</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="6"/>
-        <v>448040506.02249157</v>
+        <v>461941434.55591583</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="7"/>
-        <v>251602777395.35788</v>
+        <v>253784566369.11368</v>
       </c>
       <c r="K27" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L27" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511841061</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740875261106</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>11</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="18">
+        <f t="shared" si="13"/>
+        <v>523465010.5614683</v>
+      </c>
+      <c r="E28" s="18">
+        <f t="shared" si="10"/>
+        <v>274079634370.93893</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18">
         <f t="shared" si="11"/>
-        <v>517955456.23003626</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="10"/>
-        <v>271769408937.47235</v>
-      </c>
-      <c r="G28" s="2">
-        <f>G27*$A$14</f>
-        <v>6555835568.1924181</v>
-      </c>
-      <c r="H28" s="11">
-        <f>H27*$A$14</f>
-        <v>3662416873475.5527</v>
+        <v>6761864383.4781132</v>
+      </c>
+      <c r="H28" s="19">
+        <f t="shared" si="12"/>
+        <v>3701374441169.9556</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="6"/>
-        <v>6037880111.9623814</v>
+        <v>6238399372.9166451</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="7"/>
-        <v>3390647464538.0806</v>
+        <v>3427294806799.0166</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172819</v>
+        <v>13.504740874595687</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511222409</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874644963</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>12</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="18">
+        <f t="shared" si="13"/>
+        <v>7069259324.5501251</v>
+      </c>
+      <c r="E29" s="18">
+        <f t="shared" si="10"/>
+        <v>3701374441170.9556</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18">
         <f t="shared" si="11"/>
-        <v>6980067440.3683167</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="10"/>
-        <v>3662416873476.5527</v>
-      </c>
-      <c r="G29" s="2">
-        <f>G28*$A$14</f>
-        <v>88347702188.555084</v>
-      </c>
-      <c r="H29" s="11">
-        <f>H28*$A$14</f>
-        <v>49355434843124.219</v>
+        <v>91317226328.029648</v>
+      </c>
+      <c r="H29" s="19">
+        <f t="shared" si="12"/>
+        <v>49986102707851.672</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" si="6"/>
-        <v>81367634748.186768</v>
+        <v>84247967003.479523</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="7"/>
-        <v>45693017969647.664</v>
+        <v>46284728266680.719</v>
       </c>
       <c r="K29" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172822</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="9"/>
-        <v>13.4761925111765</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874599337</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>13</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="18">
+        <f t="shared" si="13"/>
+        <v>95468515353.368774</v>
+      </c>
+      <c r="E30" s="18">
+        <f t="shared" si="10"/>
+        <v>49986102707852.672</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18">
         <f t="shared" si="11"/>
-        <v>94064732567.372742</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="shared" si="10"/>
-        <v>49355434843125.219</v>
-      </c>
-      <c r="G30" s="2">
-        <f>G29*$A$14</f>
-        <v>1190590642612.7327</v>
-      </c>
-      <c r="H30" s="11">
-        <f>H29*$A$14</f>
-        <v>665123341418588.75</v>
+        <v>1233215478946.8474</v>
+      </c>
+      <c r="H30" s="19">
+        <f t="shared" si="12"/>
+        <v>675049364400462.75</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" si="6"/>
-        <v>1096525910045.3599</v>
+        <v>1137746963593.4785</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="7"/>
-        <v>615767906575463.5</v>
+        <v>625063261692610.13</v>
       </c>
       <c r="K30" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.504740874595687</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511173094</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.50474087459596</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>14</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="18">
+        <f t="shared" si="13"/>
+        <v>1289277561529.6052</v>
+      </c>
+      <c r="E31" s="18">
+        <f t="shared" si="10"/>
+        <v>675049364400463.75</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18">
         <f t="shared" si="11"/>
-        <v>1267634444589.9026</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="10"/>
-        <v>665123341418589.75</v>
-      </c>
-      <c r="G31" s="2">
-        <f>G30*$A$14</f>
-        <v>16044628701850.145</v>
-      </c>
-      <c r="H31" s="11">
-        <f>H30*$A$14</f>
-        <v>8963330192631429</v>
+        <v>16654255485717.588</v>
+      </c>
+      <c r="H31" s="19">
+        <f t="shared" si="12"/>
+        <v>9116366743788768</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="6"/>
-        <v>14776994257260.242</v>
+        <v>15364977924187.982</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="7"/>
-        <v>8298206851212839</v>
+        <v>8441317379388304</v>
       </c>
       <c r="K31" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172822</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L31" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172842</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874595706</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>15</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="18">
+        <f t="shared" si="13"/>
+        <v>17411359383887.918</v>
+      </c>
+      <c r="E32" s="18">
+        <f t="shared" si="10"/>
+        <v>9116366743788768</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18">
         <f t="shared" si="11"/>
-        <v>17082885809087.164</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="10"/>
-        <v>8963330192631430</v>
-      </c>
-      <c r="G32" s="2">
-        <f>G31*$A$14</f>
-        <v>216220505156421.41</v>
-      </c>
-      <c r="H32" s="11">
-        <f>H31*$A$14</f>
-        <v>1.207915632171089E+17</v>
+        <v>224911404793929.78</v>
+      </c>
+      <c r="H32" s="19">
+        <f t="shared" si="12"/>
+        <v>1.2311417059264898E+17</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="6"/>
-        <v>199137619347334.25</v>
+        <v>207500045410041.88</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="7"/>
-        <v>1.1182823302447747E+17</v>
+        <v>1.1399780384886021E+17</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.50474087459569</v>
       </c>
       <c r="L32" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172822</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.50474087459569</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>16</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="18">
+        <f t="shared" si="13"/>
+        <v>235135896753866.38</v>
+      </c>
+      <c r="E33" s="18">
+        <f t="shared" si="10"/>
+        <v>1.2311417059264898E+17</v>
+      </c>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18">
         <f t="shared" si="11"/>
-        <v>230212257809640.91</v>
-      </c>
-      <c r="E33" s="3">
-        <f t="shared" si="10"/>
-        <v>1.207915632171089E+17</v>
-      </c>
-      <c r="G33" s="2">
-        <f>G32*$A$14</f>
-        <v>2913829152350970.5</v>
-      </c>
-      <c r="H33" s="11">
-        <f>H32*$A$14</f>
-        <v>1.6278103596392612E+18</v>
+        <v>3037370241483320</v>
+      </c>
+      <c r="H33" s="19">
+        <f t="shared" si="12"/>
+        <v>1.6626249718444931E+18</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="6"/>
-        <v>2683616894541329.5</v>
+        <v>2802234344729453.5</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" si="7"/>
-        <v>1.5070187964221522E+18</v>
+        <v>1.5395108012518441E+18</v>
       </c>
       <c r="K33" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.504740874595687</v>
       </c>
       <c r="L33" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172819</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874595688</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>17</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="18">
+        <f t="shared" si="13"/>
+        <v>3175449355976651</v>
+      </c>
+      <c r="E34" s="18">
+        <f t="shared" si="10"/>
+        <v>1.6626249718444931E+18</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18">
         <f t="shared" si="11"/>
-        <v>3102384704674469.5</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" si="10"/>
-        <v>1.6278103596392612E+18</v>
-      </c>
-      <c r="G34" s="2">
-        <f>G33*$A$14</f>
-        <v>3.92673226017492E+16</v>
-      </c>
-      <c r="H34" s="11">
-        <f>H33*$A$14</f>
-        <v>2.1936685778180149E+19</v>
+        <v>4.1018898051440368E+16</v>
+      </c>
+      <c r="H34" s="19">
+        <f t="shared" si="12"/>
+        <v>2.2453319416391832E+19</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="6"/>
-        <v>3.6164937897074728E+16</v>
+        <v>3.784344869546372E+16</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" si="7"/>
-        <v>2.0308875418540888E+19</v>
+        <v>2.0790694444547338E+19</v>
       </c>
       <c r="K34" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.50474087459569</v>
       </c>
       <c r="L34" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172822</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874595688</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>18</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="18">
+        <f t="shared" si="13"/>
+        <v>4.2883620712866432E+16</v>
+      </c>
+      <c r="E35" s="18">
+        <f t="shared" si="10"/>
+        <v>2.2453319416391832E+19</v>
+      </c>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18">
         <f t="shared" si="11"/>
-        <v>4.1808333523911192E+16</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="10"/>
-        <v>2.1936685778180149E+19</v>
-      </c>
-      <c r="G35" s="2">
-        <f>G34*$A$14</f>
-        <v>5.2917399877949984E+17</v>
-      </c>
-      <c r="H35" s="11">
-        <f>H34*$A$14</f>
-        <v>2.9562300060386263E+20</v>
+        <v>5.5394958914616019E+17</v>
+      </c>
+      <c r="H35" s="19">
+        <f t="shared" si="12"/>
+        <v>3.0322626049289978E+20</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="6"/>
-        <v>4.8736566525558867E+17</v>
+        <v>5.1106596843329376E+17</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" si="7"/>
-        <v>2.7368631482568249E+20</v>
+        <v>2.8077294107650795E+20</v>
       </c>
       <c r="K35" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172822</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L35" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172821</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874595688</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>19</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="18">
+        <f t="shared" si="13"/>
+        <v>5.791321854917056E+17</v>
+      </c>
+      <c r="E36" s="18">
+        <f t="shared" si="10"/>
+        <v>3.0322626049289978E+20</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18">
         <f t="shared" si="11"/>
-        <v>5.6341715113954758E+17</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="10"/>
-        <v>2.9562300060386263E+20</v>
-      </c>
-      <c r="G36" s="2">
-        <f>G35*$A$14</f>
-        <v>7.131250679459671E+18</v>
-      </c>
-      <c r="H36" s="11">
-        <f>H35*$A$14</f>
-        <v>3.9838724668682121E+21</v>
+        <v>7.4809456590076375E+18</v>
+      </c>
+      <c r="H36" s="19">
+        <f t="shared" si="12"/>
+        <v>4.0949920743292634E+21</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" si="6"/>
-        <v>6.5678335283201239E+18</v>
+        <v>6.9018134735159316E+18</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="7"/>
-        <v>3.6882494662643496E+21</v>
+        <v>3.7917658138363639E+21</v>
       </c>
       <c r="K36" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L36" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172822</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+        <v>13.504740874595688</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>20</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="18">
+        <f t="shared" si="13"/>
+        <v>7.8210300972037683E+18</v>
+      </c>
+      <c r="E37" s="18">
+        <f t="shared" si="10"/>
+        <v>4.0949920743292634E+21</v>
+      </c>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18">
         <f t="shared" si="11"/>
-        <v>7.5927179928530964E+18</v>
-      </c>
-      <c r="E37" s="3">
-        <f t="shared" si="10"/>
-        <v>3.9838724668682121E+21</v>
-      </c>
-      <c r="G37" s="2">
-        <f>G36*$A$14</f>
-        <v>9.6102107001830506E+19</v>
-      </c>
-      <c r="H37" s="11">
-        <f>H36*$A$14</f>
-        <v>5.3687432303476988E+22</v>
+        <v>1.0102823262182962E+20</v>
+      </c>
+      <c r="H37" s="19">
+        <f t="shared" si="12"/>
+        <v>5.5301806847339788E+22</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" si="6"/>
-        <v>8.8509389008977412E+19</v>
+        <v>9.3207202524625846E+19</v>
       </c>
       <c r="J37" s="3">
         <f t="shared" si="7"/>
-        <v>4.9703559836608775E+22</v>
+        <v>5.1206814773010521E+22</v>
       </c>
       <c r="K37" s="4">
         <f t="shared" si="8"/>
-        <v>13.476192511172821</v>
+        <v>13.504740874595688</v>
       </c>
       <c r="L37" s="4">
         <f t="shared" si="9"/>
-        <v>13.476192511172819</v>
+        <v>13.504740874595687</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="B14:L14"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -3873,6 +3915,235 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD4DCC49-AC74-45CF-AE7C-0FF7AD14A271}">
+  <dimension ref="B3:N8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="J3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="M3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="J4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.0389999999999997</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3275</v>
+      </c>
+      <c r="E6" s="5">
+        <f>D6</f>
+        <v>3275</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8.1440000000000001</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5653</v>
+      </c>
+      <c r="H6" s="5">
+        <f>G6</f>
+        <v>5653</v>
+      </c>
+      <c r="J6" s="5">
+        <f>F6/C6</f>
+        <v>1.348567643649611</v>
+      </c>
+      <c r="K6" s="5">
+        <f>H6/D6</f>
+        <v>1.7261068702290077</v>
+      </c>
+      <c r="M6" s="5">
+        <f>J6/$B6</f>
+        <v>0.44952254788320367</v>
+      </c>
+      <c r="N6" s="5">
+        <f>K6/$B6</f>
+        <v>0.57536895674300259</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>54.212000000000003</v>
+      </c>
+      <c r="D7" s="5">
+        <v>29946</v>
+      </c>
+      <c r="E7" s="5">
+        <f>D7-D6</f>
+        <v>26671</v>
+      </c>
+      <c r="F7" s="5">
+        <v>101.53700000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <v>69805</v>
+      </c>
+      <c r="H7" s="5">
+        <f>G7-G6</f>
+        <v>64152</v>
+      </c>
+      <c r="J7" s="5">
+        <f>F7/C7</f>
+        <v>1.8729617058953738</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" ref="K7:K8" si="0">H7/D7</f>
+        <v>2.1422560609096375</v>
+      </c>
+      <c r="M7" s="5">
+        <f>J7/$B7</f>
+        <v>0.46824042647384345</v>
+      </c>
+      <c r="N7" s="5">
+        <f>K7/$B7</f>
+        <v>0.53556401522740937</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>901.01599999999996</v>
+      </c>
+      <c r="D8" s="5">
+        <v>491954</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8-D7</f>
+        <v>462008</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2139.73</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1539469</v>
+      </c>
+      <c r="H8" s="5">
+        <f>G8-G7</f>
+        <v>1469664</v>
+      </c>
+      <c r="J8" s="5">
+        <f>F8/C8</f>
+        <v>2.3747968959485739</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>2.9874012610935168</v>
+      </c>
+      <c r="M8" s="5">
+        <f>J8/$B8</f>
+        <v>0.47495937918971476</v>
+      </c>
+      <c r="N8" s="5">
+        <f>K8/$B8</f>
+        <v>0.59748025221870338</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="F4:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5D1B85-54A7-4B62-9796-2CEA5F0D08DB}">
   <dimension ref="A3:E22"/>
   <sheetViews>
@@ -3880,13 +4151,13 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>17</v>
       </c>
@@ -3900,7 +4171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>261</v>
       </c>
@@ -3915,14 +4186,14 @@
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3501</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>3240</v>
       </c>
       <c r="E5">
@@ -3930,14 +4201,14 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>46740</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>43239</v>
       </c>
       <c r="E6">
@@ -3945,14 +4216,14 @@
         <v>43239</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>621648</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>574908</v>
       </c>
       <c r="E7">
@@ -3960,14 +4231,14 @@
         <v>574908</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8448873.8365633115</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>7618438</v>
       </c>
       <c r="E8">
@@ -3975,14 +4246,14 @@
         <v>7827225.8365633115</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>114829403.62739694</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>100803036</v>
       </c>
       <c r="E9">
@@ -3990,14 +4261,14 @@
         <v>106380529.79083362</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1560656744.6138043</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>1332343288</v>
       </c>
       <c r="E10">
@@ -4005,14 +4276,14 @@
         <v>1445827340.9864073</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>21211026074.922855</v>
       </c>
       <c r="C11">
         <v>9</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>17596479795</v>
       </c>
       <c r="E11">
@@ -4020,14 +4291,14 @@
         <v>19650369330.309052</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>288280961655.27423</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>232248063316</v>
       </c>
       <c r="E12">
@@ -4035,14 +4306,14 @@
         <v>267069935580.35138</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3918052458157.2817</v>
       </c>
       <c r="C13">
         <v>11</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>3063288809012</v>
       </c>
       <c r="E13">
@@ -4050,14 +4321,14 @@
         <v>3629771496502.0073</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>53250603080855.453</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>40374425656248</v>
       </c>
       <c r="E14">
@@ -4065,14 +4336,14 @@
         <v>49332550622698.172</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>723733732194195.63</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>531653418284628</v>
       </c>
       <c r="E15">
@@ -4080,14 +4351,14 @@
         <v>670483129113340.13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9836330197433046</v>
       </c>
       <c r="C16">
         <v>14</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>6989320578825350</v>
       </c>
       <c r="E16">
@@ -4095,14 +4366,14 @@
         <v>9112596465238850</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.3368644772104101E+17</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>9.1365146187124304E+16</v>
       </c>
       <c r="E17">
@@ -4110,14 +4381,14 @@
         <v>1.2385011752360797E+17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.8169445256051533E+18</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>1.1E+18</v>
       </c>
       <c r="E18">
@@ -4125,14 +4396,14 @@
         <v>1.6832580778841124E+18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.4694256339395154E+19</v>
       </c>
       <c r="C19">
         <v>17</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <v>1.2E+19</v>
       </c>
       <c r="E19">
@@ -4140,14 +4411,14 @@
         <v>2.2877311813789999E+19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3.3562185722354683E+20</v>
       </c>
       <c r="C20">
         <v>18</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>2.9E+19</v>
       </c>
       <c r="E20">
@@ -4155,14 +4426,14 @@
         <v>3.1092760088415168E+20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4.5614668244324959E+21</v>
       </c>
       <c r="C21">
         <v>19</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <v>1.5E+18</v>
       </c>
       <c r="E21">
@@ -4170,14 +4441,14 @@
         <v>4.2258449672089491E+21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6.1995305557645563E+22</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="13">
         <v>490000000</v>
       </c>
       <c r="E22">
@@ -4191,7 +4462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537A84A7-1C83-4D40-B5AF-0FBCC0BD07B5}">
   <dimension ref="B2:D8"/>
   <sheetViews>
@@ -4199,9 +4470,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -4212,7 +4483,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>Data!B4</f>
         <v>1</v>
@@ -4226,7 +4497,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>Data!B5</f>
         <v>2</v>
@@ -4240,7 +4511,7 @@
         <v>0.46700000000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>Data!B6</f>
         <v>3</v>
@@ -4254,7 +4525,7 @@
         <v>6.5449999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>Data!B7</f>
         <v>4</v>
@@ -4268,7 +4539,7 @@
         <v>87.323999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>Data!B8</f>
         <v>5</v>
@@ -4282,7 +4553,7 @@
         <v>1149.732</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>Data!B9</f>
         <v>6</v>

</xml_diff>

<commit_message>
Memory logging from full run through
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Tree Generator.xlsx
+++ b/Dissertation/Research/Tree Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Will Garside\Documents\Projects\Active\CubeSolver\Dissertation\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20207AD8-8616-4AE3-B178-A580ED48869C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2CFA07-28B8-4615-9541-A1C254910300}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A08C0A5D-9DC9-4B70-9FA4-56456CBF2D01}"/>
   </bookViews>
@@ -111,10 +111,10 @@
     <t>All Positions</t>
   </si>
   <si>
-    <t>Dup:All Factor</t>
+    <t>Factor/Depth</t>
   </si>
   <si>
-    <t>Factor/Depth</t>
+    <t>All/Dup Factor</t>
   </si>
 </sst>
 </file>
@@ -3919,7 +3919,7 @@
   <dimension ref="B3:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3942,11 +3942,11 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="J3" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K3" s="14"/>
       <c r="M3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N3" s="14"/>
     </row>

</xml_diff>